<commit_message>
Changes TO Renewal Case
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/uploadAddedVIN_CA_SELECT.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/uploadAddedVIN_CA_SELECT.xlsx
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B5"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1136,16 +1136,16 @@
         <v>39</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="AG5" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="AH5" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="AI5">
         <v>20190101</v>

</xml_diff>